<commit_message>
Add hint and popup columns
</commit_message>
<xml_diff>
--- a/scenarios/cough/processes/APICalmer.xlsx
+++ b/scenarios/cough/processes/APICalmer.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t xml:space="preserve">Output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Popup</t>
   </si>
   <si>
     <t xml:space="preserve">calmer </t>
@@ -271,7 +277,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -282,6 +288,10 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -442,19 +452,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.38671875" defaultRowHeight="14.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.39453125" defaultRowHeight="14.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="48.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="32.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="32.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="45.61"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.15"/>
@@ -482,130 +492,136 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="72.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="E2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
-      <c r="B3" s="9"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>17</v>
+      <c r="D4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>19</v>
+      <c r="A5" s="6"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="145.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="B6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="C6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="B7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="D7" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>30</v>
       </c>
+      <c r="F7" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="22"/>
     </row>
     <row r="9" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="22"/>
     </row>
     <row r="10" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="21"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="22"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>